<commit_message>
reset password api and map
</commit_message>
<xml_diff>
--- a/Documentations/ElephantAPIMap.xlsx
+++ b/Documentations/ElephantAPIMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gen10\BackToWork\Elephant\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8C0A6E4-54E9-41B2-9BE9-9B1DAA15C415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA206CA2-8B7E-41AE-9127-098A480D6DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-170" windowWidth="19420" windowHeight="10420" xr2:uid="{F5CE9F15-1EDA-4B88-A2B1-3580F6E17EAD}"/>
+    <workbookView xWindow="18560" yWindow="340" windowWidth="23020" windowHeight="11080" xr2:uid="{F5CE9F15-1EDA-4B88-A2B1-3580F6E17EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>GET</t>
   </si>
@@ -669,6 +669,32 @@
   </si>
   <si>
     <t>Departure</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/resetPassword/{id} - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resets a password to a new random default password</t>
+    </r>
+  </si>
+  <si>
+    <t>User (w/ reset PW)</t>
   </si>
 </sst>
 </file>
@@ -716,7 +742,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -785,11 +811,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,12 +843,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,6 +865,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC055CB-F276-43DA-A2C4-91C328551D93}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,26 +1201,26 @@
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1196,7 +1234,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1208,7 +1246,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1220,7 +1258,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1232,7 +1270,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1282,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1256,7 +1294,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1306,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1280,7 +1318,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1298,7 +1336,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1312,7 +1350,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1325,7 +1363,7 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1372,7 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1346,7 +1384,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1396,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
@@ -1370,159 +1408,171 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A23" s="16" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="A33" s="8"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+      <c r="A34" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="B34" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A13:A19"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Checking for default password map and impl
</commit_message>
<xml_diff>
--- a/Documentations/ElephantAPIMap.xlsx
+++ b/Documentations/ElephantAPIMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gen10\BackToWork\Elephant\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA206CA2-8B7E-41AE-9127-098A480D6DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BD97C0-7FB3-45E7-BAFF-13090CE1D6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18560" yWindow="340" windowWidth="23020" windowHeight="11080" xr2:uid="{F5CE9F15-1EDA-4B88-A2B1-3580F6E17EAD}"/>
+    <workbookView xWindow="19110" yWindow="-150" windowWidth="19380" windowHeight="10380" xr2:uid="{F5CE9F15-1EDA-4B88-A2B1-3580F6E17EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>GET</t>
   </si>
@@ -505,6 +505,175 @@
     </r>
   </si>
   <si>
+    <t>ADMIN - /api/admin</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>User []</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Role []</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/departures/{id} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- returns a list of departures for the current day</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>by location id</t>
+    </r>
+  </si>
+  <si>
+    <t>Location []</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/flagged/{id} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- returns a list of users flagged as isAuthorized=false by location id</t>
+    </r>
+  </si>
+  <si>
+    <t>User - firstname, lastname, email, location, role</t>
+  </si>
+  <si>
+    <t>PV - userId</t>
+  </si>
+  <si>
+    <t>PV - locId</t>
+  </si>
+  <si>
+    <t>(PV = PathVariable)</t>
+  </si>
+  <si>
+    <t>Path Description</t>
+  </si>
+  <si>
+    <t>PV - locId, PV - capacity</t>
+  </si>
+  <si>
+    <t>Edited Location</t>
+  </si>
+  <si>
+    <t>Created user</t>
+  </si>
+  <si>
+    <t>Edited user</t>
+  </si>
+  <si>
+    <t>PV - locId, PV - increment</t>
+  </si>
+  <si>
+    <t>/timeInterval/{id}{time}{time}</t>
+  </si>
+  <si>
+    <t>PV - locId, PV - startTime (Time object), PV - endTime</t>
+  </si>
+  <si>
+    <t>USER - /api/user</t>
+  </si>
+  <si>
+    <t>TimeSlot []</t>
+  </si>
+  <si>
+    <t>Input - all need "email" &amp; "password" header</t>
+  </si>
+  <si>
+    <t>User - userId, password</t>
+  </si>
+  <si>
+    <t>Attendance - isAttending, User</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>PV - timeSlotId; User</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/resetPassword/{id} - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resets a password to a new random default password</t>
+    </r>
+  </si>
+  <si>
+    <t>User (w/ reset PW)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -524,177 +693,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- creates an attendence entry for the user id from an attendence object (isAttending, userId)</t>
-    </r>
-  </si>
-  <si>
-    <t>ADMIN - /api/admin</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>User []</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Role []</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">/departures/{id} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- returns a list of departures for the current day</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>by location id</t>
-    </r>
-  </si>
-  <si>
-    <t>Location []</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/flagged/{id} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- returns a list of users flagged as isAuthorized=false by location id</t>
-    </r>
-  </si>
-  <si>
-    <t>User - firstname, lastname, email, location, role</t>
-  </si>
-  <si>
-    <t>PV - userId</t>
-  </si>
-  <si>
-    <t>PV - locId</t>
-  </si>
-  <si>
-    <t>(PV = PathVariable)</t>
-  </si>
-  <si>
-    <t>Path Description</t>
-  </si>
-  <si>
-    <t>PV - locId, PV - capacity</t>
-  </si>
-  <si>
-    <t>Edited Location</t>
-  </si>
-  <si>
-    <t>Created user</t>
-  </si>
-  <si>
-    <t>Edited user</t>
-  </si>
-  <si>
-    <t>PV - locId, PV - increment</t>
-  </si>
-  <si>
-    <t>/timeInterval/{id}{time}{time}</t>
-  </si>
-  <si>
-    <t>PV - locId, PV - startTime (Time object), PV - endTime</t>
-  </si>
-  <si>
-    <t>USER - /api/user</t>
-  </si>
-  <si>
-    <t>TimeSlot []</t>
-  </si>
-  <si>
-    <t>Input - all need "email" &amp; "password" header</t>
-  </si>
-  <si>
-    <t>User - userId, password</t>
-  </si>
-  <si>
-    <t>Attendance - isAttending, User</t>
-  </si>
-  <si>
-    <t>Attendance</t>
-  </si>
-  <si>
-    <t>PV - timeSlotId; User</t>
-  </si>
-  <si>
-    <t>Arrival</t>
-  </si>
-  <si>
-    <t>Departure</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/resetPassword/{id} - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>resets a password to a new random default password</t>
-    </r>
-  </si>
-  <si>
-    <t>User (w/ reset PW)</t>
+      <t>- creates an attendence entry for the user from an attendence object</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>/checkChange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - checks to make sure that the user has changed their password from the default</t>
+    </r>
+  </si>
+  <si>
+    <t>Boolean (true if hasChanged)</t>
   </si>
 </sst>
 </file>
@@ -742,7 +760,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -822,11 +840,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -847,6 +891,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,7 +910,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC055CB-F276-43DA-A2C4-91C328551D93}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,142 +1241,142 @@
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
     <col min="2" max="2" width="86.5546875" customWidth="1"/>
     <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1336,34 +1386,34 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1372,51 +1422,51 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1433,146 +1483,159 @@
         <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
     </row>
     <row r="25" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="4" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="4" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="A34" s="8"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
+      <c r="A35" s="13" t="s">
+        <v>2</v>
+      </c>
       <c r="B35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A28:A32"/>
+  <mergeCells count="7">
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>